<commit_message>
sound system works completely now
</commit_message>
<xml_diff>
--- a/The Agency/Assets/Story_Sheet.xlsx
+++ b/The Agency/Assets/Story_Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>TYPE</t>
   </si>
@@ -60,6 +60,27 @@
   </si>
   <si>
     <t>£</t>
+  </si>
+  <si>
+    <t>audiotest</t>
+  </si>
+  <si>
+    <t>AUDIO</t>
+  </si>
+  <si>
+    <t>KitchenCounterCoins</t>
+  </si>
+  <si>
+    <t>LivingRoomTablePour</t>
+  </si>
+  <si>
+    <t>audiotest2</t>
+  </si>
+  <si>
+    <t>audiotest3</t>
+  </si>
+  <si>
+    <t>KitchenStove</t>
   </si>
 </sst>
 </file>
@@ -417,22 +438,22 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -452,10 +473,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -464,20 +485,20 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <f>(LEN(D2)*0.03)</f>
+        <f t="shared" ref="E2:E37" si="0">(LEN(D2)*0.03)</f>
         <v>1.02</v>
       </c>
       <c r="F2">
-        <f>E2+C2</f>
+        <f t="shared" ref="F2:F37" si="1">E2+C2</f>
         <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -486,385 +507,418 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <f>(LEN(D3)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>1.53</v>
       </c>
       <c r="F3">
-        <f>E3+C3</f>
+        <f t="shared" si="1"/>
         <v>6.53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E4">
-        <f>(LEN(D4)*0.03)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F4">
-        <f>E4+C4</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E5">
-        <f>(LEN(D5)*0.03)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F5">
-        <f>E5+C5</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.57</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E6">
-        <f>(LEN(D6)*0.03)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.36</v>
       </c>
       <c r="F6">
-        <f>E6+C6</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.3600000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="E7">
-        <f>(LEN(D7)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>E7+C7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="E8">
-        <f>(LEN(D8)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>E8+C8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="E9">
-        <f>(LEN(D9)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>E9+C9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="E10">
-        <f>(LEN(D10)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>E10+C10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11">
-        <f>(LEN(D11)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f>E11+C11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12">
-        <f>(LEN(D12)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>E12+C12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="E13">
-        <f>(LEN(D13)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>E13+C13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14">
-        <f>(LEN(D14)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>E14+C14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15">
-        <f>(LEN(D15)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>E15+C15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16">
-        <f>(LEN(D16)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>E16+C16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17">
-        <f>(LEN(D17)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17">
-        <f>E17+C17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18">
-        <f>(LEN(D18)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f>E18+C18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19">
-        <f>(LEN(D19)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19">
-        <f>E19+C19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20">
-        <f>(LEN(D20)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20">
-        <f>E20+C20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21">
-        <f>(LEN(D21)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21">
-        <f>E21+C21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22">
-        <f>(LEN(D22)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22">
-        <f>E22+C22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23">
-        <f>(LEN(D23)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23">
-        <f>E23+C23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24">
-        <f>(LEN(D24)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F24">
-        <f>E24+C24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25">
-        <f>(LEN(D25)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F25">
-        <f>E25+C25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26">
-        <f>(LEN(D26)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>E26+C26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27">
-        <f>(LEN(D27)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f>E27+C27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28">
-        <f>(LEN(D28)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F28">
-        <f>E28+C28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29">
-        <f>(LEN(D29)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F29">
-        <f>E29+C29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30">
-        <f>(LEN(D30)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F30">
-        <f>E30+C30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31">
-        <f>(LEN(D31)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f>E31+C31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32">
-        <f>(LEN(D32)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F32">
-        <f>E32+C32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33">
-        <f>(LEN(D33)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F33">
-        <f>E33+C33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34">
-        <f>(LEN(D34)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f>E34+C34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35">
-        <f>(LEN(D35)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f>E35+C35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36">
-        <f>(LEN(D36)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f>E36+C36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37">
-        <f>(LEN(D37)*0.03)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f>E37+C37</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rooms! and text! and a choice! things! Progress!
</commit_message>
<xml_diff>
--- a/The Agency/Assets/Story_Sheet.xlsx
+++ b/The Agency/Assets/Story_Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>TYPE</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>KitchenStove</t>
+  </si>
+  <si>
+    <t>ROOM</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -435,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +457,7 @@
     <col min="4" max="4" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,16 +471,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -484,16 +496,19 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E37" si="0">(LEN(D2)*0.03)</f>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <f>(LEN(D2)*0.03)</f>
         <v>1.02</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F37" si="1">E2+C2</f>
+      <c r="G2">
+        <f>F2+C2</f>
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -506,16 +521,19 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <f>(LEN(D3)*0.03)</f>
         <v>1.53</v>
       </c>
-      <c r="F3">
-        <f t="shared" si="1"/>
+      <c r="G3">
+        <f>F3+C3</f>
         <v>6.53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -528,16 +546,19 @@
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <f>(LEN(D4)*0.03)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
+      <c r="G4">
+        <f>F4+C4</f>
         <v>3.57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -550,16 +571,19 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <f>(LEN(D5)*0.03)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
+      <c r="G5">
+        <f>F5+C5</f>
         <v>5.57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -572,357 +596,360 @@
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <f>(LEN(D6)*0.03)</f>
         <v>0.36</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
+      <c r="G6">
+        <f>F6+C6</f>
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D7)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>F7+C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D8)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>F8+C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D9)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>F9+C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D10)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>F10+C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D11)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>F11+C11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D12)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>F12+C12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D13)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>F13+C13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D14)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>F14+C14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(LEN(D15)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>F15+C15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D16)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>F16+C16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D17)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>F17+C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D18)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>F18+C18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D19)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>F19+C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D20)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>F20+C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D21)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>F21+C21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D22)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>F22+C22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D23)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>F23+C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D24)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>F24+C24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D25)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>F25+C25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D26)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>F26+C26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D27)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>F27+C27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D28)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f>F28+C28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D29)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f>F29+C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D30)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>F30+C30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D31)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>F31+C31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D32)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f>F32+C32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D33)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f>F33+C33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D34)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f>F34+C34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D35)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f>F35+C35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D36)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>F36+C36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="F37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+        <f>(LEN(D37)*0.03)</f>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f>F37+C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
     </row>
   </sheetData>

</xml_diff>